<commit_message>
Test cases added for signyourslf,signup and contacts pages
</commit_message>
<xml_diff>
--- a/tests/TestData/Contactbookready.xlsx
+++ b/tests/TestData/Contactbookready.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\OpenSign_automation_new\OpenSign-Tests\tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Phone</t>
   </si>
@@ -35,37 +35,22 @@
     <t>email</t>
   </si>
   <si>
-    <t>fvvxcv</t>
-  </si>
-  <si>
-    <t>dffddf</t>
-  </si>
-  <si>
-    <t>pravin+otpver@nxglabs.in</t>
-  </si>
-  <si>
-    <t>dfsdfsf</t>
-  </si>
-  <si>
-    <t>asdadasd</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>JKKKRR</t>
-  </si>
-  <si>
-    <t>Pravin+Jemsbonddd@nxgalsb.in</t>
-  </si>
-  <si>
-    <t>pravin+karlosebreed@nxglabs.in</t>
-  </si>
-  <si>
-    <t>pravin+NirmalaVaman552333///#@nxglabs.in</t>
-  </si>
-  <si>
-    <t>pravin+Nirmala343455dd#@//@nxglabs.in</t>
+    <t>Mathew Karl</t>
+  </si>
+  <si>
+    <t>mathew@nxglabs.in</t>
+  </si>
+  <si>
+    <t>Tony Stark</t>
+  </si>
+  <si>
+    <t>tonys@nxglabs.in</t>
+  </si>
+  <si>
+    <t>Andy amaya</t>
+  </si>
+  <si>
+    <t>andyamaya@nxglabs.in</t>
   </si>
 </sst>
 </file>
@@ -400,7 +385,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -426,52 +411,41 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>34343434</v>
+        <v>35534343434</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>343434</v>
+        <v>233343434</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>67546546</v>
+        <v>3367546546</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
@@ -486,13 +460,6 @@
       <c r="B9" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new test cases added for request signature E2E flow
</commit_message>
<xml_diff>
--- a/tests/TestData/Contactbookready.xlsx
+++ b/tests/TestData/Contactbookready.xlsx
@@ -47,10 +47,10 @@
     <t>tonys@nxglabs.in</t>
   </si>
   <si>
-    <t>Andy amaya</t>
-  </si>
-  <si>
-    <t>andyamaya@nxglabs.in</t>
+    <t>Steve Head</t>
+  </si>
+  <si>
+    <t>stevehead@nxglabs.in</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -436,7 +436,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>3367546546</v>
+        <v>336746546</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -460,6 +460,9 @@
       <c r="B9" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>